<commit_message>
just for some tests
</commit_message>
<xml_diff>
--- a/TestThreeMachine.xlsx
+++ b/TestThreeMachine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Johnson'sRule\OM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C28C3E7-F318-416D-B11B-BF753BF40862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21B37E2-F04B-4529-A6BC-06563D8D4EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Job</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -37,22 +37,6 @@
   <si>
     <t>machine 2</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>machine3</t>
@@ -394,7 +378,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -410,12 +394,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -428,8 +412,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -442,8 +426,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -456,8 +440,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5">
         <v>1</v>

</xml_diff>